<commit_message>
shift update on frontend
</commit_message>
<xml_diff>
--- a/bluetyk-frontend-App/public/excels/upload_template.xlsx
+++ b/bluetyk-frontend-App/public/excels/upload_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>slno</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>xxxxxx</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>morning shift</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,9 +442,10 @@
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,8 +482,11 @@
       <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -507,8 +517,11 @@
       <c r="L2" t="s">
         <v>17</v>
       </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
     </row>
   </sheetData>

</xml_diff>